<commit_message>
fixed excel stuff and added other stuff
</commit_message>
<xml_diff>
--- a/Uipath/Academy2/Sample Columns.xlsx
+++ b/Uipath/Academy2/Sample Columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/Training/HoldenNicole-Code/HoldenNicole-Code/Uipath/Academy2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{9756652C-E32B-49AB-958E-9DABA14A796A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75BDCA84-518E-46D2-8CFD-F4E7103BAD8F}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{9756652C-E32B-49AB-958E-9DABA14A796A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2CF97259-ECBC-4C51-816C-EDC999C03668}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1030" windowWidth="12290" windowHeight="9120" xr2:uid="{8E5E89D9-C451-4BD2-B571-51F01044F859}"/>
   </bookViews>
@@ -380,93 +380,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7076718E-B0FB-4DEB-8B81-43BDEF0BADE4}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>50</v>
       </c>
       <c r="B1">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>30</v>
       </c>
       <c r="B2">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>9086</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>90</v>
       </c>
       <c r="B3">
         <v>8996</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>43</v>
       </c>
       <c r="B4">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1234</v>
       </c>
       <c r="B5">
         <v>324</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>95585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6643</v>
       </c>
       <c r="B6">
         <v>88942</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>7537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3213</v>
       </c>
       <c r="B8">
         <v>4324</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>7775</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7732</v>
       </c>
       <c r="B9">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>952</v>
       </c>
       <c r="B10">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>3668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3577</v>
       </c>

</xml_diff>